<commit_message>
ADT_A04 Channel with in built Mappers
</commit_message>
<xml_diff>
--- a/V2-messages/ADT_A04/A04_Patient_Delago.xlsx
+++ b/V2-messages/ADT_A04/A04_Patient_Delago.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\project_surabhi\HL7-v2\V2-messages\ADT_A01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\project_surabhi\HL7-v2\V2-messages\ADT_A04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978AEEB1-D0CE-42F2-8B38-7CEB38687D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CA288E-DF77-47E8-B6C2-E77DBA2F127E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="A01_Patient_Delago" sheetId="2" r:id="rId1"/>
+    <sheet name="A04_Patient_Delago" sheetId="2" r:id="rId1"/>
     <sheet name="Table" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A01_Patient_Delago!$A$1:$F$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A04_Patient_Delago!$A$1:$F$114</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="1181">
   <si>
     <t>MSH.1</t>
   </si>
@@ -4169,8 +4169,8 @@
   <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5940,7 +5940,7 @@
   <dimension ref="B1:E299"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>